<commit_message>
Update Test Cases (Menu, MenuItem, MenuSection, MenuItemOptions, ShopDB).xlsx
</commit_message>
<xml_diff>
--- a/docs/contributions/AthanasiaZ/Writing-Charts/Phase6/Test Cases (Menu, MenuItem, MenuSection, MenuItemOptions, ShopDB).xlsx
+++ b/docs/contributions/AthanasiaZ/Writing-Charts/Phase6/Test Cases (Menu, MenuItem, MenuSection, MenuItemOptions, ShopDB).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\git-ΤΛ\nomnomr\docs\contributions\AthanasiaZ\Writing-Charts\Phase6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{296EAEEA-BD16-4FC3-A7B8-4B0BD2AB72E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D735C94B-CA18-496A-BCD2-A8A1540FECA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9560D621-A71A-4FED-9B46-A878053B0129}"/>
   </bookViews>
@@ -188,7 +188,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,13 +205,25 @@
       <charset val="161"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF56E39F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -226,9 +238,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -241,12 +252,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF56E39F"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -558,7 +577,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,186 +592,189 @@
     <col min="8" max="8" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="E3" s="4" t="s">
+      <c r="A3" s="4"/>
+      <c r="E3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="4" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>22</v>
       </c>
     </row>
+    <row r="7" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:8" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>36</v>
       </c>
     </row>
+    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:8" ht="89.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="3" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>